<commit_message>
Fixed typos on tests
</commit_message>
<xml_diff>
--- a/src/tests/data/results/IEEE14_con_results.xlsx
+++ b/src/tests/data/results/IEEE14_con_results.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Vm_br_failure" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Va_br_failure" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Vm" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Va" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="branch_id" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Info" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
@@ -223,35 +223,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,7 +447,7 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,7 +527,7 @@
       <c r="B2" s="5" t="n">
         <v>1.06</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="0" t="n">
         <v>1.06</v>
       </c>
       <c r="D2" s="6" t="n">
@@ -595,7 +595,7 @@
       <c r="B3" s="5" t="n">
         <v>1.045</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="0" t="n">
         <v>1.045</v>
       </c>
       <c r="D3" s="6" t="n">
@@ -663,7 +663,7 @@
       <c r="B4" s="5" t="n">
         <v>1.01</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="0" t="n">
         <v>1.01</v>
       </c>
       <c r="D4" s="6" t="n">
@@ -731,7 +731,7 @@
       <c r="B5" s="5" t="n">
         <v>1.0168</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="0" t="n">
         <v>1.0177</v>
       </c>
       <c r="D5" s="6" t="n">
@@ -799,8 +799,8 @@
       <c r="B6" s="5" t="n">
         <v>1.0193</v>
       </c>
-      <c r="C6" s="6" t="n">
-        <v>1.0196</v>
+      <c r="C6" s="0" t="n">
+        <v>1.0195</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>1.0065</v>
@@ -867,7 +867,7 @@
       <c r="B7" s="5" t="n">
         <v>1.07</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="0" t="n">
         <v>1.07</v>
       </c>
       <c r="D7" s="6" t="n">
@@ -935,8 +935,8 @@
       <c r="B8" s="5" t="n">
         <v>1.0592</v>
       </c>
-      <c r="C8" s="6" t="n">
-        <v>1.0616</v>
+      <c r="C8" s="0" t="n">
+        <v>1.0615</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>1.0578</v>
@@ -1003,7 +1003,7 @@
       <c r="B9" s="5" t="n">
         <v>1.09</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="0" t="n">
         <v>1.09</v>
       </c>
       <c r="D9" s="6" t="n">
@@ -1071,8 +1071,8 @@
       <c r="B10" s="5" t="n">
         <v>1.0515</v>
       </c>
-      <c r="C10" s="6" t="n">
-        <v>1.056</v>
+      <c r="C10" s="0" t="n">
+        <v>1.0559</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>1.0529</v>
@@ -1139,7 +1139,7 @@
       <c r="B11" s="5" t="n">
         <v>1.0471</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="0" t="n">
         <v>1.051</v>
       </c>
       <c r="D11" s="6" t="n">
@@ -1207,7 +1207,7 @@
       <c r="B12" s="5" t="n">
         <v>1.0547</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="0" t="n">
         <v>1.0569</v>
       </c>
       <c r="D12" s="6" t="n">
@@ -1275,7 +1275,7 @@
       <c r="B13" s="5" t="n">
         <v>1.0571</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="0" t="n">
         <v>1.0552</v>
       </c>
       <c r="D13" s="6" t="n">
@@ -1343,7 +1343,7 @@
       <c r="B14" s="5" t="n">
         <v>1.0552</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="0" t="n">
         <v>1.0504</v>
       </c>
       <c r="D14" s="6" t="n">
@@ -1411,8 +1411,8 @@
       <c r="B15" s="5" t="n">
         <v>1.0191</v>
       </c>
-      <c r="C15" s="6" t="n">
-        <v>1.0356</v>
+      <c r="C15" s="0" t="n">
+        <v>1.0355</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>1.0336</v>
@@ -1491,7 +1491,7 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2534,11 +2534,15 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.43"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2853,10 +2857,13 @@
   <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.98"/>
+  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">

</xml_diff>